<commit_message>
Fixed error in distributions tab
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Laos/2017Jun/InputForCode_LaoPDR_29Jun2017.xlsx
+++ b/input_spreadsheets/Laos/2017Jun/InputForCode_LaoPDR_29Jun2017.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Laos/2017Jun/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="800" windowWidth="25380" windowHeight="14140" tabRatio="500" firstSheet="17" activeTab="19"/>
+    <workbookView xWindow="1040" yWindow="1100" windowWidth="25380" windowHeight="14140" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -33,13 +38,13 @@
     <sheet name="Interventions mortality eff" sheetId="24" r:id="rId24"/>
     <sheet name="Interventions incidence eff" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -2115,6 +2120,62 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2446,12 +2507,12 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2459,7 +2520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2467,7 +2528,7 @@
         <v>823940</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2475,7 +2536,7 @@
         <v>174530</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -2483,7 +2544,7 @@
         <v>184299</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>71</v>
       </c>
@@ -2491,7 +2552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>70</v>
       </c>
@@ -2499,7 +2560,7 @@
         <v>0.29949999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>72</v>
       </c>
@@ -2511,11 +2572,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2527,12 +2583,12 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -2555,7 +2611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2578,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
         <v>46</v>
       </c>
@@ -2598,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
         <v>47</v>
       </c>
@@ -2618,7 +2674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="s">
         <v>48</v>
       </c>
@@ -2638,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2661,7 +2717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
         <v>46</v>
       </c>
@@ -2681,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="5" t="s">
         <v>47</v>
       </c>
@@ -2701,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>48</v>
       </c>
@@ -2721,7 +2777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2744,7 +2800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>46</v>
       </c>
@@ -2764,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
@@ -2784,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -2804,7 +2860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2827,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
@@ -2847,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>47</v>
       </c>
@@ -2867,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
@@ -2887,7 +2943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2910,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
@@ -2930,7 +2986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
@@ -2950,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="5" t="s">
         <v>48</v>
       </c>
@@ -2970,7 +3026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -2993,7 +3049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
@@ -3013,7 +3069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
@@ -3033,7 +3089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
@@ -3053,7 +3109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3076,7 +3132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="5" t="s">
         <v>46</v>
       </c>
@@ -3096,7 +3152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="5" t="s">
         <v>47</v>
       </c>
@@ -3116,7 +3172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="5" t="s">
         <v>48</v>
       </c>
@@ -3138,11 +3194,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3154,13 +3205,13 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -3177,7 +3228,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
@@ -3196,7 +3247,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -3215,7 +3266,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
@@ -3234,7 +3285,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -3253,7 +3304,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>27</v>
       </c>
@@ -3272,7 +3323,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>28</v>
       </c>
@@ -3291,7 +3342,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
         <v>54</v>
       </c>
@@ -3310,7 +3361,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>31</v>
       </c>
@@ -3329,118 +3380,113 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3452,9 +3498,9 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -3468,7 +3514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5">
         <v>45</v>
       </c>
@@ -3484,11 +3530,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3498,12 +3539,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>55</v>
       </c>
@@ -3523,7 +3564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>45</v>
       </c>
@@ -3543,7 +3584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -3563,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
@@ -3583,7 +3624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
@@ -3605,11 +3646,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3621,9 +3657,9 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -3643,7 +3679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -3665,11 +3701,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3681,9 +3712,9 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
@@ -3697,7 +3728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -3713,11 +3744,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3729,12 +3755,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -3754,7 +3780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>73</v>
       </c>
@@ -3774,7 +3800,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3782,7 +3808,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -3790,7 +3816,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -3801,11 +3827,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3817,12 +3838,12 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="70.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>78</v>
       </c>
@@ -3842,7 +3863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>57</v>
       </c>
@@ -3862,7 +3883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>58</v>
       </c>
@@ -3882,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
@@ -3902,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>60</v>
       </c>
@@ -3924,11 +3945,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3940,13 +3956,13 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="43.1640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -3966,7 +3982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>74</v>
       </c>
@@ -3986,7 +4002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>75</v>
       </c>
@@ -4006,7 +4022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4016,11 +4032,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4030,12 +4041,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -4052,7 +4063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>45</v>
       </c>
@@ -4069,14 +4080,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4085,11 +4096,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4101,13 +4107,13 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4115,7 +4121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>2017</v>
       </c>
@@ -4123,7 +4129,7 @@
         <v>174510</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2018</v>
       </c>
@@ -4131,7 +4137,7 @@
         <v>173930</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>2019</v>
       </c>
@@ -4139,7 +4145,7 @@
         <v>172990</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>2020</v>
       </c>
@@ -4147,7 +4153,7 @@
         <v>171730</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>2021</v>
       </c>
@@ -4155,7 +4161,7 @@
         <v>170200</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>2022</v>
       </c>
@@ -4163,7 +4169,7 @@
         <v>168470</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>2023</v>
       </c>
@@ -4171,7 +4177,7 @@
         <v>166600</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>2024</v>
       </c>
@@ -4179,7 +4185,7 @@
         <v>164710</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>2025</v>
       </c>
@@ -4187,7 +4193,7 @@
         <v>162880</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>2026</v>
       </c>
@@ -4195,7 +4201,7 @@
         <v>161150</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>2027</v>
       </c>
@@ -4203,7 +4209,7 @@
         <v>159540</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>2028</v>
       </c>
@@ -4211,7 +4217,7 @@
         <v>158030</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>2029</v>
       </c>
@@ -4219,7 +4225,7 @@
         <v>156640</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>2030</v>
       </c>
@@ -4230,11 +4236,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4242,11 +4243,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="37.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -4254,7 +4255,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4268,7 +4269,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -4284,7 +4285,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>75</v>
       </c>
@@ -4301,7 +4302,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>76</v>
       </c>
@@ -4318,7 +4319,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
@@ -4335,7 +4336,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -4352,7 +4353,7 @@
       <c r="F6" s="14"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -4369,91 +4370,91 @@
       <c r="F7" s="14"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1">
+    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1">
+    <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1">
+    <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:3" ht="15.75" customHeight="1">
+    <row r="25" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
@@ -4461,11 +4462,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4477,7 +4473,7 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
@@ -4487,7 +4483,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4512,7 +4508,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -4535,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>75</v>
       </c>
@@ -4558,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>76</v>
       </c>
@@ -4583,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
@@ -4606,7 +4602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -4630,7 +4626,7 @@
         <v>0.29949999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -4653,93 +4649,93 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1">
+    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1">
+    <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1">
+    <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:3" ht="15.75" customHeight="1">
+    <row r="25" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
@@ -4747,11 +4743,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4763,12 +4754,12 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4788,7 +4779,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -4808,7 +4799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>69</v>
       </c>
@@ -4827,7 +4818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -4847,7 +4838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>69</v>
       </c>
@@ -4866,11 +4857,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4882,12 +4868,12 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -4910,7 +4896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -4933,7 +4919,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -4953,34 +4939,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4992,12 +4973,12 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -5020,7 +5001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5043,7 +5024,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -5063,34 +5044,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5102,12 +5078,12 @@
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -5130,7 +5106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5153,7 +5129,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -5173,34 +5149,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5212,9 +5183,9 @@
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5225,7 +5196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>30.1</v>
       </c>
@@ -5240,11 +5211,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5256,9 +5222,9 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5278,7 +5244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5298,7 +5264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -5318,7 +5284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -5338,7 +5304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -5358,7 +5324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -5378,7 +5344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -5398,7 +5364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -5418,7 +5384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -5438,7 +5404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -5458,7 +5424,7 @@
         <v>0.19639999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -5478,7 +5444,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -5498,7 +5464,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -5518,7 +5484,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -5538,7 +5504,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -5558,7 +5524,7 @@
         <v>3.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -5578,7 +5544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -5598,7 +5564,7 @@
         <v>0.13669999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -5625,11 +5591,6 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5637,13 +5598,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -5666,7 +5627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -5689,7 +5650,7 @@
         <v>20.12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -5709,7 +5670,7 @@
         <v>27.79</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -5729,7 +5690,7 @@
         <v>29.59</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -5749,7 +5710,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>35</v>
       </c>
@@ -5772,7 +5733,7 @@
         <v>73.16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -5792,7 +5753,7 @@
         <v>21.64</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -5812,7 +5773,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -5832,7 +5793,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
@@ -5855,7 +5816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>46</v>
       </c>
@@ -5875,7 +5836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
@@ -5895,7 +5856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -5912,18 +5873,13 @@
         <v>11.7</v>
       </c>
       <c r="G13" s="25">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5935,9 +5891,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
@@ -5948,7 +5904,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5">
         <v>2.4E-2</v>
       </c>
@@ -5961,11 +5917,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5977,9 +5928,9 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -5999,7 +5950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -6019,7 +5970,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
@@ -6042,11 +5993,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6056,9 +6002,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -6081,7 +6027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -6104,7 +6050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -6124,7 +6070,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -6144,7 +6090,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -6164,7 +6110,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -6187,7 +6133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -6207,7 +6153,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -6227,7 +6173,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -6247,7 +6193,7 @@
         <v>6.39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -6270,7 +6216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
@@ -6290,7 +6236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -6310,7 +6256,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
@@ -6330,7 +6276,7 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -6353,7 +6299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
@@ -6373,7 +6319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -6393,7 +6339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
@@ -6413,7 +6359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -6436,7 +6382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
@@ -6456,7 +6402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -6476,7 +6422,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
@@ -6498,11 +6444,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6512,9 +6453,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -6537,7 +6478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -6560,7 +6501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -6580,7 +6521,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -6600,7 +6541,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -6620,7 +6561,7 @@
         <v>12.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -6643,7 +6584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -6663,7 +6604,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -6683,7 +6624,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -6703,7 +6644,7 @@
         <v>9.68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -6726,7 +6667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
@@ -6746,7 +6687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -6766,7 +6707,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
@@ -6786,7 +6727,7 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -6809,7 +6750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
@@ -6829,7 +6770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -6849,7 +6790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
@@ -6869,7 +6810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -6892,7 +6833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
@@ -6912,7 +6853,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -6932,7 +6873,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
@@ -6954,10 +6895,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>